<commit_message>
Agregando hover al tooltip
</commit_message>
<xml_diff>
--- a/Customers data/Med1.xlsx
+++ b/Customers data/Med1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
   <si>
     <t>Cte</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>PROPATO HNOS. S.A.I.C</t>
+  </si>
+  <si>
+    <t>nro_cliente</t>
   </si>
 </sst>
 </file>
@@ -505,8 +508,8 @@
   </sheetPr>
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -524,7 +527,9 @@
       <c r="D1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="9"/>
+      <c r="E1" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>

</xml_diff>